<commit_message>
12th commit: stage 2 development - almost done
</commit_message>
<xml_diff>
--- a/Questionnaire/API Coding.xlsx
+++ b/Questionnaire/API Coding.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\gitproject\nCoV monitoring\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3D68DF-7A6C-4065-8F45-C5149A724679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1FEBC3-D2E9-484C-990E-4F3AB8BD46B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="18220" windowHeight="11620" activeTab="1" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
   </bookViews>
   <sheets>
     <sheet name="Casetype" sheetId="1" r:id="rId1"/>
-    <sheet name="API parameter" sheetId="2" r:id="rId2"/>
+    <sheet name="1. Informap API parameter" sheetId="2" r:id="rId2"/>
+    <sheet name="2.Nav API return" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
   <si>
     <t>页面显示内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -297,10 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Request in Progress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>View Completed Requests</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -345,14 +342,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>根据staffid，返回用户自己团队的数据，不能搜索非自己团队的成员数据，并能提交revoke申请</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据staffid，可以搜索任意GSC员工数据，并能提交revoke申请</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>返回全部GSC的数据，但不能提交信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -381,10 +370,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>myToDoList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reviewHist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -433,6 +418,162 @@
   </si>
   <si>
     <t>CAO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Case Center</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面菜单显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Json变量mapping：case数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>totcase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonresp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>healthcase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>closecontact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hadcontact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curinhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beenhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>totreview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reviewlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viewcompletecase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>healthcase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonresp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>closecontact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hadcontact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curinhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beenhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>backhubei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Action Center</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Action History</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>只读权限，不能操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>myAction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionHist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>totaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Action Center</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionlist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回GSC全部access active的员工list，但不能提交revoke申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回用户自己团队全部access active的员工list，并能提交revoke申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回用户自己团队全部被revoke的员工list，并能提交reacitivate申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回GSC全部access revoke的员工list，但不能提交reactivate申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回全部GSC的数据，支持下钻功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回全部GSC的数据，不支持下钻功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Request in Process</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +644,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +684,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,7 +795,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -679,128 +826,125 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,188 +1275,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="20">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C2" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="22">
-        <v>1</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>97</v>
+      <c r="D4" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>97</v>
+      <c r="C5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>97</v>
+      <c r="C6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="22">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>97</v>
+      <c r="C7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>97</v>
+      <c r="C8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>97</v>
+      <c r="C9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
+      <c r="A10" s="20">
         <v>8</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>97</v>
+      <c r="C10" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="22">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>97</v>
+      <c r="C11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="22">
+      <c r="A12" s="20">
         <v>10</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="22">
+      <c r="A13" s="20">
         <v>11</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="21"/>
+      <c r="B13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="19"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
@@ -1325,11 +1469,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FF4E36-CAFF-4E81-BE35-2C52316F2330}">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1349,28 +1493,29 @@
     <col min="13" max="13" width="14.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="48" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1398,111 +1543,120 @@
       <c r="I2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="N2" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="36" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="M3" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="38"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="48" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="36"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="48"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="36"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="48"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="36"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="36"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="48"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1512,7 +1666,7 @@
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1522,167 +1676,175 @@
       <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="48"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="36"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="48"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="36"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="48"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="37"/>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="36"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="48"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="36" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="38" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="39" t="s">
+      <c r="G11" s="31"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="36"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="38"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="36"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="38"/>
       <c r="F14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="36"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1692,7 +1854,7 @@
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="36"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1702,410 +1864,430 @@
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="32"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="36"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="38"/>
       <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="35"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="36"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="38"/>
       <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="37"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="36"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="35"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="33" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="39" t="s">
+      <c r="F19" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="31"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="36"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="N19" s="47"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="46"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="47"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="38"/>
       <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="46"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="36"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" s="32"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="47"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="38"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="46"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="47"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="38"/>
       <c r="B23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="46"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="32"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="47"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="38"/>
       <c r="B24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="46"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="47"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
       <c r="B25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="46"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="32"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="47"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="38"/>
       <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="47"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="47"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="33" t="s">
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="35" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J27" s="32" t="s">
+      <c r="G27" s="31"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J27" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="K27" s="39" t="s">
+      <c r="K27" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="L27" s="42"/>
-      <c r="M27" s="45" t="s">
+      <c r="L27" s="47"/>
+      <c r="M27" s="42" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
+      <c r="N27" s="47"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="38"/>
       <c r="B28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="36"/>
       <c r="F28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="37"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="46"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="47"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="38"/>
       <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="36"/>
       <c r="F29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="37"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="46"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="47"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
       <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="46"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="47"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="38"/>
       <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="38"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="46"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="47"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="38"/>
       <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="37"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="46"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="47"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="38"/>
       <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="38"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="46"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="47"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="38"/>
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="34"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="47"/>
-    </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="G34" s="33"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="47"/>
+    </row>
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
@@ -2122,263 +2304,303 @@
         <v>51</v>
       </c>
       <c r="H35" s="7"/>
-      <c r="I35" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J35" s="12" t="s">
+      <c r="I35" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="M35" s="12" t="s">
+      <c r="M35" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A36" s="36" t="s">
+      <c r="N35" s="17"/>
+    </row>
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
+      <c r="A36" s="38" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="33" t="s">
+      <c r="C36" s="14"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" s="15"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J36" s="12" t="s">
+      <c r="G36" s="14"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="K36" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="L36" s="19"/>
-      <c r="M36" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N36" s="17"/>
+    </row>
+    <row r="37" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="38"/>
       <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="38"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="36"/>
       <c r="F37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" s="35"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="L37" s="7"/>
-      <c r="M37" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
+      <c r="M37" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="N37" s="17"/>
+    </row>
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A38" s="38"/>
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="36"/>
       <c r="F38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="N38" s="7"/>
+    </row>
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A39" s="38"/>
+      <c r="B39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K39" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-    </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="2" t="s">
+      <c r="L39" s="17"/>
+      <c r="M39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N39" s="17"/>
+    </row>
+    <row r="40" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A40" s="38"/>
+      <c r="B40" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="2" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="L39" s="19"/>
-      <c r="M39" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="12" t="s">
+      <c r="G40" s="16"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="L40" s="17"/>
+      <c r="M40" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N40" s="17"/>
+    </row>
+    <row r="41" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+      <c r="A41" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="31"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K41" s="40"/>
+      <c r="L41" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="M41" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N41" s="17"/>
+    </row>
+    <row r="42" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L40" s="19"/>
-      <c r="M40" s="12" t="s">
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42" s="33"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" s="40"/>
+      <c r="L42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="N42" s="17"/>
+    </row>
+    <row r="43" spans="1:14" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A41" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="30"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="K41" s="30"/>
-      <c r="L41" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M41" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G42" s="31"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="K42" s="31"/>
-      <c r="L42" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="M42" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-    </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-    </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-    </row>
-    <row r="46" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-    </row>
-    <row r="47" spans="1:13" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="N43" s="49"/>
+    </row>
+    <row r="44" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A44" s="37"/>
+      <c r="B44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="N44" s="49"/>
+    </row>
+    <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2863,7 +3085,63 @@
       <c r="I91" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="70">
+    <mergeCell ref="N19:N26"/>
+    <mergeCell ref="N27:N34"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="I11:I18"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J19:J26"/>
+    <mergeCell ref="K19:K26"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="L19:L26"/>
+    <mergeCell ref="M19:M26"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="M27:M34"/>
+    <mergeCell ref="J11:J18"/>
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="K11:K18"/>
+    <mergeCell ref="L11:L18"/>
+    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="N3:N10"/>
+    <mergeCell ref="N11:N18"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="H27:H34"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="G19:G26"/>
+    <mergeCell ref="H19:H26"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="E19:E26"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A10"/>
@@ -2878,59 +3156,154 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="G19:G26"/>
-    <mergeCell ref="H19:H26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="H27:H34"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J11:J18"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="K3:K10"/>
-    <mergeCell ref="L3:L10"/>
-    <mergeCell ref="M3:M10"/>
-    <mergeCell ref="K11:K18"/>
-    <mergeCell ref="L11:L18"/>
-    <mergeCell ref="M11:M18"/>
-    <mergeCell ref="L19:L26"/>
-    <mergeCell ref="M19:M26"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="K27:K34"/>
-    <mergeCell ref="M27:M34"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="H36:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J19:J26"/>
-    <mergeCell ref="K19:K26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9597A6B-B129-438A-85AB-15C154C6BADF}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="29.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="45"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="45"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" s="45"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="46"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="45"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="45"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
13th commit: fix some bugs of post json processing
</commit_message>
<xml_diff>
--- a/Questionnaire/API Coding.xlsx
+++ b/Questionnaire/API Coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\gitproject\nCoV monitoring\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1FEBC3-D2E9-484C-990E-4F3AB8BD46B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA60338-AF7E-41B7-9B8E-8ABEDA5DFEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="18220" windowHeight="11620" activeTab="1" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
   </bookViews>
   <sheets>
     <sheet name="Casetype" sheetId="1" r:id="rId1"/>
@@ -889,6 +889,42 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,53 +934,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1472,8 +1472,8 @@
   <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1494,26 +1494,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="41" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1560,103 +1560,103 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="38" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="42" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="42" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="41" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="38"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="48"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="38"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="48"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="48"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1676,175 +1676,175 @@
       <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="48"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="38"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="48"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="41"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="38"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="48"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="38"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="48"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="38" t="s">
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="42" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="42" t="s">
+      <c r="G11" s="43"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="48" t="s">
+      <c r="J11" s="39"/>
+      <c r="K11" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="38"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="38"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="38"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1854,7 +1854,7 @@
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1864,428 +1864,428 @@
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="38"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="38"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="42" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="35" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="42" t="s">
+      <c r="G19" s="43"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="48" t="s">
+      <c r="K19" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="L19" s="47"/>
-      <c r="M19" s="42" t="s">
+      <c r="L19" s="36"/>
+      <c r="M19" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="N19" s="47"/>
+      <c r="N19" s="36"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="43" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="47"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="43" t="s">
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="47"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="36"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="43" t="s">
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="47"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="36"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="43" t="s">
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="47"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="36"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="43" t="s">
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="47"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="36"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="38"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="43" t="s">
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="47"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="36"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="43" t="s">
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="47"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="36"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="35" t="s">
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="37" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="42" t="s">
+      <c r="G27" s="43"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J27" s="42" t="s">
+      <c r="J27" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="K27" s="48" t="s">
+      <c r="K27" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="L27" s="47"/>
-      <c r="M27" s="42" t="s">
+      <c r="L27" s="36"/>
+      <c r="M27" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="N27" s="47"/>
+      <c r="N27" s="36"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="38"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="36"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="47"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="36"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="38"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="36"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="47"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="36"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="36"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="47"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="36"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="36"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="47"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="36"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="38"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="36"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="46"/>
       <c r="F32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="47"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="36"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="38"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="36"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="47"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="36"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="38"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="37"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="33"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="47"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="36"/>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
@@ -2322,23 +2322,23 @@
       <c r="N35" s="17"/>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="42" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="35" t="s">
+      <c r="D36" s="43"/>
+      <c r="E36" s="37" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="42" t="s">
+      <c r="H36" s="39"/>
+      <c r="I36" s="40" t="s">
         <v>85</v>
       </c>
       <c r="J36" s="11" t="s">
@@ -2354,19 +2354,19 @@
       <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="38"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C37" s="14"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="36"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="42"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="40"/>
       <c r="J37" s="11" t="s">
         <v>129</v>
       </c>
@@ -2380,19 +2380,19 @@
       <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A38" s="38"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="15"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="36"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G38" s="15"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="42"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="40"/>
       <c r="J38" s="11" t="s">
         <v>132</v>
       </c>
@@ -2406,19 +2406,19 @@
       <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A39" s="38"/>
+      <c r="A39" s="42"/>
       <c r="B39" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C39" s="15"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="36"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="6" t="s">
         <v>70</v>
       </c>
       <c r="G39" s="15"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="42"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40"/>
       <c r="J39" s="11" t="s">
         <v>76</v>
       </c>
@@ -2432,19 +2432,19 @@
       <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A40" s="38"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="37"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="42"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="40"/>
       <c r="J40" s="11" t="s">
         <v>78</v>
       </c>
@@ -2458,29 +2458,29 @@
       <c r="N40" s="17"/>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="37" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="35" t="s">
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="G41" s="31"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="42" t="s">
+      <c r="G41" s="43"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="40" t="s">
         <v>85</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K41" s="40"/>
+      <c r="K41" s="39"/>
       <c r="L41" s="11" t="s">
         <v>87</v>
       </c>
@@ -2490,23 +2490,23 @@
       <c r="N41" s="17"/>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="37"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="37"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="38"/>
       <c r="F42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="33"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="42"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
       <c r="J42" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K42" s="40"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="11" t="s">
         <v>88</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="N42" s="17"/>
     </row>
     <row r="43" spans="1:14" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="37" t="s">
         <v>120</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2524,10 +2524,10 @@
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="31" t="s">
         <v>128</v>
       </c>
       <c r="G43" s="7"/>
@@ -2541,16 +2541,16 @@
       <c r="M43" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N43" s="49"/>
+      <c r="N43" s="35"/>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="37"/>
+      <c r="E44" s="38"/>
       <c r="F44" s="2" t="s">
         <v>125</v>
       </c>
@@ -2565,7 +2565,7 @@
       <c r="M44" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N44" s="49"/>
+      <c r="N44" s="35"/>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
@@ -3086,43 +3086,22 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="N19:N26"/>
-    <mergeCell ref="N27:N34"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J19:J26"/>
-    <mergeCell ref="K19:K26"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="H36:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="L19:L26"/>
-    <mergeCell ref="M19:M26"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="K27:K34"/>
-    <mergeCell ref="M27:M34"/>
-    <mergeCell ref="J11:J18"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="K3:K10"/>
-    <mergeCell ref="L3:L10"/>
-    <mergeCell ref="M3:M10"/>
-    <mergeCell ref="K11:K18"/>
-    <mergeCell ref="L11:L18"/>
-    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="H8:H10"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="N3:N10"/>
     <mergeCell ref="N11:N18"/>
@@ -3139,23 +3118,44 @@
     <mergeCell ref="C19:C26"/>
     <mergeCell ref="D19:D26"/>
     <mergeCell ref="G19:G26"/>
+    <mergeCell ref="J11:J18"/>
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="K11:K18"/>
+    <mergeCell ref="L11:L18"/>
+    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="L19:L26"/>
+    <mergeCell ref="M19:M26"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="M27:M34"/>
     <mergeCell ref="H19:H26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="I11:I18"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="N19:N26"/>
+    <mergeCell ref="N27:N34"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J19:J26"/>
+    <mergeCell ref="K19:K26"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C41:C42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3186,7 +3186,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="32" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -3250,7 +3250,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="32" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -3266,13 +3266,13 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="32" t="s">
         <v>127</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="33"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -3281,25 +3281,25 @@
       <c r="B13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="33"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" s="45"/>
+      <c r="C14" s="33"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="34"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="33"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="45"/>
+      <c r="C17" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
14th commit: access control feature added
</commit_message>
<xml_diff>
--- a/Questionnaire/API Coding.xlsx
+++ b/Questionnaire/API Coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\gitproject\nCoV monitoring\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA60338-AF7E-41B7-9B8E-8ABEDA5DFEAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB499F-4E3D-4A1A-B836-86A963C0665B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
   </bookViews>
   <sheets>
     <sheet name="Casetype" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="137">
   <si>
     <t>页面显示内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -574,6 +574,10 @@
   </si>
   <si>
     <t>Request in Process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有权限，可以操作</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -795,7 +799,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -901,50 +905,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,6 +962,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2781300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>33483</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A683013-3C64-4C81-9EBC-074A194DDBC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="27071" t="5740" r="23552" b="14658"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4381500" y="47625"/>
+          <a:ext cx="3886200" cy="2890983"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1471,9 +1520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FF4E36-CAFF-4E81-BE35-2C52316F2330}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1494,26 +1543,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="47" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1560,103 +1609,103 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="42" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="35" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="J3" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="46" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="42"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="41"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="42"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="46"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="42"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1666,7 +1715,7 @@
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1676,60 +1725,60 @@
       <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="41"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="42"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="41"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="42"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="35"/>
       <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="41"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="38"/>
@@ -1739,112 +1788,112 @@
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="42"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="41"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="42" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="35" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40" t="s">
+      <c r="G11" s="39"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="39"/>
-      <c r="K11" s="41" t="s">
+      <c r="J11" s="44"/>
+      <c r="K11" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="44"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="42"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1854,7 +1903,7 @@
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="42"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1864,60 +1913,60 @@
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="40"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="42"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="42"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
@@ -1927,365 +1976,365 @@
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="42"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="37" t="s">
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="36" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40" t="s">
+      <c r="G19" s="39"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J19" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="40" t="s">
+      <c r="L19" s="48"/>
+      <c r="M19" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="N19" s="36"/>
+      <c r="N19" s="48"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="46"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="36"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="48"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="42"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="46"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="44"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="36"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="48"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="46"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="36"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="48"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="42"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="46"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="36"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="48"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="42"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="46"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="36"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="48"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="46"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="36"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="48"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="38"/>
       <c r="F26" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="36"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="48"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="35" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="37" t="s">
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="36" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40" t="s">
+      <c r="G27" s="39"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="J27" s="40" t="s">
+      <c r="J27" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="L27" s="36"/>
-      <c r="M27" s="40" t="s">
+      <c r="L27" s="48"/>
+      <c r="M27" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="N27" s="36"/>
+      <c r="N27" s="48"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="46"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="36"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="46"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="44"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="36"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="48"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="46"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="44"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="36"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="48"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="46"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G31" s="44"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="36"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="42"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="46"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="44"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="36"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="48"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="42"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="46"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="37"/>
       <c r="F33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="44"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="36"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="48"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
       <c r="E34" s="38"/>
       <c r="F34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="45"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="36"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="48"/>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
@@ -2322,23 +2371,23 @@
       <c r="N35" s="17"/>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="37" t="s">
+      <c r="D36" s="39"/>
+      <c r="E36" s="36" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="40" t="s">
+      <c r="H36" s="44"/>
+      <c r="I36" s="47" t="s">
         <v>85</v>
       </c>
       <c r="J36" s="11" t="s">
@@ -2354,19 +2403,19 @@
       <c r="N36" s="17"/>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="42"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C37" s="14"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="46"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="37"/>
       <c r="F37" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="47"/>
       <c r="J37" s="11" t="s">
         <v>129</v>
       </c>
@@ -2380,19 +2429,19 @@
       <c r="N37" s="17"/>
     </row>
     <row r="38" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A38" s="42"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="15"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="46"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G38" s="15"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="47"/>
       <c r="J38" s="11" t="s">
         <v>132</v>
       </c>
@@ -2406,19 +2455,19 @@
       <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A39" s="42"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C39" s="15"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="46"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="6" t="s">
         <v>70</v>
       </c>
       <c r="G39" s="15"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="47"/>
       <c r="J39" s="11" t="s">
         <v>76</v>
       </c>
@@ -2432,19 +2481,19 @@
       <c r="N39" s="17"/>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="45"/>
+      <c r="D40" s="41"/>
       <c r="E40" s="38"/>
       <c r="F40" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="40"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="47"/>
       <c r="J40" s="11" t="s">
         <v>78</v>
       </c>
@@ -2458,29 +2507,29 @@
       <c r="N40" s="17"/>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="37" t="s">
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="36" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="40" t="s">
+      <c r="G41" s="39"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="47" t="s">
         <v>85</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K41" s="39"/>
+      <c r="K41" s="44"/>
       <c r="L41" s="11" t="s">
         <v>87</v>
       </c>
@@ -2494,19 +2543,19 @@
       <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
       <c r="E42" s="38"/>
       <c r="F42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="45"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="40"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="47"/>
       <c r="J42" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K42" s="39"/>
+      <c r="K42" s="44"/>
       <c r="L42" s="11" t="s">
         <v>88</v>
       </c>
@@ -2516,7 +2565,7 @@
       <c r="N42" s="17"/>
     </row>
     <row r="43" spans="1:14" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2524,7 +2573,7 @@
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="37" t="s">
+      <c r="E43" s="36" t="s">
         <v>124</v>
       </c>
       <c r="F43" s="31" t="s">
@@ -2541,9 +2590,11 @@
       <c r="M43" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N43" s="35"/>
-    </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="N43" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A44" s="38"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
@@ -2565,7 +2616,9 @@
       <c r="M44" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="N44" s="35"/>
+      <c r="N44" s="11" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A45" s="13"/>
@@ -3086,6 +3139,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="N19:N26"/>
+    <mergeCell ref="N27:N34"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J19:J26"/>
+    <mergeCell ref="K19:K26"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="H36:H40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="I11:I18"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="I36:I40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="L19:L26"/>
+    <mergeCell ref="M19:M26"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="M27:M34"/>
+    <mergeCell ref="H19:H26"/>
+    <mergeCell ref="J11:J18"/>
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="K11:K18"/>
+    <mergeCell ref="L11:L18"/>
+    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="N3:N10"/>
+    <mergeCell ref="N11:N18"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="H27:H34"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="G19:G26"/>
     <mergeCell ref="A19:A26"/>
     <mergeCell ref="E19:E26"/>
     <mergeCell ref="C11:C14"/>
@@ -3102,60 +3209,6 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="N3:N10"/>
-    <mergeCell ref="N11:N18"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="H27:H34"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="G19:G26"/>
-    <mergeCell ref="J11:J18"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="K3:K10"/>
-    <mergeCell ref="L3:L10"/>
-    <mergeCell ref="M3:M10"/>
-    <mergeCell ref="K11:K18"/>
-    <mergeCell ref="L11:L18"/>
-    <mergeCell ref="M11:M18"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="L19:L26"/>
-    <mergeCell ref="M19:M26"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="K27:K34"/>
-    <mergeCell ref="M27:M34"/>
-    <mergeCell ref="H19:H26"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="N19:N26"/>
-    <mergeCell ref="N27:N34"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J19:J26"/>
-    <mergeCell ref="K19:K26"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="H36:H40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="C41:C42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3167,14 +3220,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9597A6B-B129-438A-85AB-15C154C6BADF}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
@@ -3272,7 +3327,6 @@
       <c r="B12" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="33"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
@@ -3281,7 +3335,6 @@
       <c r="B13" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="33"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C14" s="33"/>
@@ -3305,5 +3358,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17th commit: fix more bugs
</commit_message>
<xml_diff>
--- a/Questionnaire/API Coding.xlsx
+++ b/Questionnaire/API Coding.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\gitproject\nCoV monitoring\Questionnaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB499F-4E3D-4A1A-B836-86A963C0665B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF3EE53-AD56-4B4B-992D-1B80324B3CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{8EBD710D-A346-46AE-8DD1-450CE71AA270}"/>
   </bookViews>
   <sheets>
-    <sheet name="Casetype" sheetId="1" r:id="rId1"/>
+    <sheet name="Casetype" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="1. Informap API parameter" sheetId="2" r:id="rId2"/>
     <sheet name="2.Nav API return" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="142">
   <si>
     <t>页面显示内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -509,10 +509,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>backhubei</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>My Action Center</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -578,6 +574,27 @@
   </si>
   <si>
     <t>有权限，可以操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outside GZ/FS</t>
+  </si>
+  <si>
+    <t>Outside GZ/FS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current in Hubei/Oversea</t>
+  </si>
+  <si>
+    <t>Been in Hubei/Oversea</t>
+  </si>
+  <si>
+    <t>Outside GZ or FS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>outsidework</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -905,25 +922,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -932,24 +964,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1013,7 +1030,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1520,9 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FF4E36-CAFF-4E81-BE35-2C52316F2330}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1535,34 +1552,35 @@
     <col min="6" max="6" width="21.25" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" customWidth="1"/>
-    <col min="10" max="10" width="14.75" customWidth="1"/>
-    <col min="11" max="11" width="17.375" customWidth="1"/>
-    <col min="12" max="12" width="15.875" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
+    <col min="9" max="9" width="27.25" customWidth="1"/>
+    <col min="10" max="10" width="14.75" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.75" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="45" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1605,107 +1623,107 @@
         <v>58</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="35" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="41" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="47" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="K3" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="N3" s="46" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="46"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="46"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="35"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="46"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="37"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1733,7 @@
       <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="35"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
@@ -1725,84 +1743,84 @@
       <c r="H7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="46"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="46"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="40"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="35"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="46"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="40"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="38"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="35"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="46"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
@@ -1811,89 +1829,89 @@
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="35" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="47" t="s">
+      <c r="G11" s="42"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="46" t="s">
+      <c r="J11" s="38"/>
+      <c r="K11" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="44"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="35"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="44"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="35"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1903,7 +1921,7 @@
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1913,430 +1931,430 @@
       <c r="H15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="47"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="44"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="35"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="44"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="37"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="35"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="44"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="35"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="44"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="44"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="47" t="s">
+      <c r="G19" s="42"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="47" t="s">
+      <c r="J19" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="47" t="s">
+      <c r="L19" s="35"/>
+      <c r="M19" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="N19" s="48"/>
+      <c r="N19" s="35"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="31" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="48"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="35"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="35"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="31" t="s">
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="48"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="35"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="31" t="s">
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="40"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="48"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="48"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="35"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="35"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="40"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="48"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="35"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="35"/>
-      <c r="B25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="37"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="40"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="48"/>
+        <v>141</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="35"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="31" t="s">
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G26" s="41"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="48"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="35"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="41" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="36" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="39"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="47" t="s">
+      <c r="G27" s="42"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="J27" s="47" t="s">
+      <c r="J27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="K27" s="46" t="s">
+      <c r="K27" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="L27" s="48"/>
-      <c r="M27" s="47" t="s">
+      <c r="L27" s="35"/>
+      <c r="M27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N27" s="48"/>
+      <c r="N27" s="35"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="37"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="46"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="48"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="35"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="37"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="48"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="35"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="37"/>
+        <v>138</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="48"/>
+        <v>138</v>
+      </c>
+      <c r="G30" s="43"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="35"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="37"/>
+        <v>139</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="40"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="48"/>
+        <v>139</v>
+      </c>
+      <c r="G31" s="43"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="35"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
-      <c r="B32" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="40"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="48"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="43"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="35"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="37"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="40"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="48"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="35"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="38"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="37"/>
       <c r="F34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="41"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="48"/>
-    </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="G34" s="44"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="35"/>
+    </row>
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
@@ -2370,15 +2388,15 @@
       </c>
       <c r="N35" s="17"/>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A36" s="35" t="s">
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="39"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="36" t="s">
         <v>67</v>
       </c>
@@ -2386,8 +2404,8 @@
         <v>68</v>
       </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="47" t="s">
+      <c r="H36" s="38"/>
+      <c r="I36" s="39" t="s">
         <v>85</v>
       </c>
       <c r="J36" s="11" t="s">
@@ -2402,72 +2420,72 @@
       </c>
       <c r="N36" s="17"/>
     </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="35"/>
+    <row r="37" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="41"/>
       <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C37" s="14"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="37"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="45"/>
       <c r="F37" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G37" s="14"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="47"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
       <c r="J37" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="K37" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="L37" s="7"/>
       <c r="M37" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N37" s="17"/>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A38" s="35"/>
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="41"/>
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="15"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="37"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G38" s="15"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="47"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="39"/>
       <c r="J38" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L38" s="7"/>
       <c r="M38" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A39" s="35"/>
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="41"/>
       <c r="B39" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" s="15"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="37"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="45"/>
       <c r="F39" s="6" t="s">
         <v>70</v>
       </c>
       <c r="G39" s="15"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="47"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="39"/>
       <c r="J39" s="11" t="s">
         <v>76</v>
       </c>
@@ -2480,20 +2498,20 @@
       </c>
       <c r="N39" s="17"/>
     </row>
-    <row r="40" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
-      <c r="A40" s="35"/>
+    <row r="40" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="41"/>
       <c r="B40" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="38"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="37"/>
       <c r="F40" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="47"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
       <c r="J40" s="11" t="s">
         <v>78</v>
       </c>
@@ -2506,30 +2524,30 @@
       </c>
       <c r="N40" s="17"/>
     </row>
-    <row r="41" spans="1:14" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="36" t="s">
         <v>83</v>
       </c>
       <c r="F41" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="G41" s="39"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="47" t="s">
+      <c r="G41" s="42"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="39" t="s">
         <v>85</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="K41" s="44"/>
+      <c r="K41" s="38"/>
       <c r="L41" s="11" t="s">
         <v>87</v>
       </c>
@@ -2538,24 +2556,24 @@
       </c>
       <c r="N41" s="17"/>
     </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" ht="40.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
+    <row r="42" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
       <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="38"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="37"/>
       <c r="F42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G42" s="41"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="47"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="39"/>
       <c r="J42" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="K42" s="44"/>
+      <c r="K42" s="38"/>
       <c r="L42" s="11" t="s">
         <v>88</v>
       </c>
@@ -2564,9 +2582,9 @@
       </c>
       <c r="N42" s="17"/>
     </row>
-    <row r="43" spans="1:14" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>81</v>
@@ -2574,50 +2592,50 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K43" s="23"/>
       <c r="L43" s="23"/>
       <c r="M43" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="37"/>
       <c r="B44" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="38"/>
+      <c r="E44" s="37"/>
       <c r="F44" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
       <c r="J44" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
       <c r="M44" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
@@ -3139,6 +3157,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="E19:E26"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="E11:E18"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="N3:N10"/>
+    <mergeCell ref="N11:N18"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="C27:C34"/>
+    <mergeCell ref="D27:D34"/>
+    <mergeCell ref="E27:E34"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="H27:H34"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="D19:D26"/>
+    <mergeCell ref="G19:G26"/>
+    <mergeCell ref="J11:J18"/>
+    <mergeCell ref="J3:J10"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="L3:L10"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="K11:K18"/>
+    <mergeCell ref="L11:L18"/>
+    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="L19:L26"/>
+    <mergeCell ref="M19:M26"/>
+    <mergeCell ref="L27:L34"/>
+    <mergeCell ref="J27:J34"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="M27:M34"/>
+    <mergeCell ref="H19:H26"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="I11:I18"/>
+    <mergeCell ref="I19:I26"/>
+    <mergeCell ref="I27:I34"/>
+    <mergeCell ref="I36:I40"/>
     <mergeCell ref="N19:N26"/>
     <mergeCell ref="N27:N34"/>
     <mergeCell ref="A43:A44"/>
@@ -3155,60 +3227,6 @@
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="C41:C42"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="I11:I18"/>
-    <mergeCell ref="I19:I26"/>
-    <mergeCell ref="I27:I34"/>
-    <mergeCell ref="I36:I40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="L19:L26"/>
-    <mergeCell ref="M19:M26"/>
-    <mergeCell ref="L27:L34"/>
-    <mergeCell ref="J27:J34"/>
-    <mergeCell ref="K27:K34"/>
-    <mergeCell ref="M27:M34"/>
-    <mergeCell ref="H19:H26"/>
-    <mergeCell ref="J11:J18"/>
-    <mergeCell ref="J3:J10"/>
-    <mergeCell ref="K3:K10"/>
-    <mergeCell ref="L3:L10"/>
-    <mergeCell ref="M3:M10"/>
-    <mergeCell ref="K11:K18"/>
-    <mergeCell ref="L11:L18"/>
-    <mergeCell ref="M11:M18"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="N3:N10"/>
-    <mergeCell ref="N11:N18"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="C27:C34"/>
-    <mergeCell ref="D27:D34"/>
-    <mergeCell ref="E27:E34"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="H27:H34"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="D19:D26"/>
-    <mergeCell ref="G19:G26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="E19:E26"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="E11:E18"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="H8:H10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3220,8 +3238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9597A6B-B129-438A-85AB-15C154C6BADF}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3241,7 +3259,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="19" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -3282,7 +3300,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>105</v>
@@ -3290,22 +3308,22 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="19" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -3321,11 +3339,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
-        <v>127</v>
+      <c r="A12" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3333,7 +3351,7 @@
         <v>81</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>